<commit_message>
Hyperlink references Side menu
</commit_message>
<xml_diff>
--- a/supplementary/S1_Table.xlsx
+++ b/supplementary/S1_Table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maylis\Dropbox\Systematic review\Supplementary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5891D578-EF3C-4779-80EF-7628C1A94063}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78939F5E-669E-4797-B5B9-4BE962E9A73B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1884" yWindow="3156" windowWidth="17280" windowHeight="9060" tabRatio="486" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="372" windowWidth="23256" windowHeight="12696" tabRatio="486" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ST1" sheetId="9" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="732" uniqueCount="213">
   <si>
     <t>Beyer et al., 2011</t>
   </si>
@@ -653,9 +653,6 @@
   </si>
   <si>
     <t>2004 - 2017</t>
-  </si>
-  <si>
-    <t>1990 - 2012</t>
   </si>
   <si>
     <t>2012 - 2015</t>
@@ -728,6 +725,9 @@
   </si>
   <si>
     <t xml:space="preserve">S1 Table. General characteristics of the included studies. </t>
+  </si>
+  <si>
+    <t>1986 - 2012</t>
   </si>
 </sst>
 </file>
@@ -1152,8 +1152,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94AB10A6-7D24-4AA8-BCD3-D79C2FDBC725}">
   <dimension ref="A1:I64"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E59" sqref="E59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1172,7 +1172,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C1" s="2"/>
     </row>
@@ -1298,7 +1298,7 @@
         <v>71</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>23</v>
@@ -1726,22 +1726,22 @@
         <v>23</v>
       </c>
       <c r="B26" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="F26" s="8" t="s">
         <v>204</v>
       </c>
-      <c r="C26" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="D26" s="7" t="s">
-        <v>211</v>
-      </c>
-      <c r="E26" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="F26" s="8" t="s">
-        <v>205</v>
-      </c>
       <c r="G26" s="23" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -1841,13 +1841,13 @@
         <v>28</v>
       </c>
       <c r="B31" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="D31" s="7" t="s">
         <v>208</v>
-      </c>
-      <c r="C31" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="D31" s="7" t="s">
-        <v>209</v>
       </c>
       <c r="E31" s="7" t="s">
         <v>99</v>
@@ -1856,7 +1856,7 @@
         <v>23</v>
       </c>
       <c r="G31" s="23" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
@@ -2031,7 +2031,7 @@
         <v>54</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E39" s="7" t="s">
         <v>23</v>
@@ -2146,7 +2146,7 @@
         <v>54</v>
       </c>
       <c r="D44" s="7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E44" s="7" t="s">
         <v>126</v>
@@ -2494,7 +2494,7 @@
         <v>152</v>
       </c>
       <c r="E59" s="11" t="s">
-        <v>200</v>
+        <v>212</v>
       </c>
       <c r="F59" s="11" t="s">
         <v>23</v>
@@ -2517,7 +2517,7 @@
         <v>103</v>
       </c>
       <c r="E60" s="11" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F60" s="11" t="s">
         <v>77</v>
@@ -2574,7 +2574,7 @@
     </row>
     <row r="64" spans="1:7" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A64" s="24" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
   </sheetData>

</xml_diff>